<commit_message>
initial setup with data
</commit_message>
<xml_diff>
--- a/excel/section.xlsx
+++ b/excel/section.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +698,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>